<commit_message>
Pulumi environment set up
</commit_message>
<xml_diff>
--- a/template-config.xlsx
+++ b/template-config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad2e409c2b6f214a/Documents/developments/azureappservice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{49EECD3D-F20A-44B7-A4FE-9FC6E6DDB728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E90B5DA-64DD-4E9B-BC47-854200F4BDF5}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{49EECD3D-F20A-44B7-A4FE-9FC6E6DDB728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BFDDEC8-91F3-4B24-B277-9B15293AB49A}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="2010" windowWidth="27675" windowHeight="10995" xr2:uid="{B647DB2F-C2DE-4079-AEE5-AABAE0DA86BE}"/>
   </bookViews>
@@ -38,22 +38,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Tenant</t>
-  </si>
-  <si>
     <t>Subscription</t>
   </si>
   <si>
-    <t>xxx</t>
-  </si>
-  <si>
-    <t>yyy</t>
-  </si>
-  <si>
     <t>Pulumi Resource Group</t>
   </si>
   <si>
-    <t>zzz</t>
+    <t>Azure subscription 1</t>
+  </si>
+  <si>
+    <t>rg-pulumi-nvtst</t>
+  </si>
+  <si>
+    <t>Pulumi Storage Account</t>
+  </si>
+  <si>
+    <t>stpuluminvtst</t>
   </si>
 </sst>
 </file>
@@ -408,12 +408,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Getting Azure resources built!
</commit_message>
<xml_diff>
--- a/template-config.xlsx
+++ b/template-config.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad2e409c2b6f214a/Documents/developments/azureappservice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{49EECD3D-F20A-44B7-A4FE-9FC6E6DDB728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BFDDEC8-91F3-4B24-B277-9B15293AB49A}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{49EECD3D-F20A-44B7-A4FE-9FC6E6DDB728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF122C7C-8B2E-484C-A354-80EA6230AD0E}"/>
   <bookViews>
     <workbookView xWindow="1065" yWindow="2010" windowWidth="27675" windowHeight="10995" xr2:uid="{B647DB2F-C2DE-4079-AEE5-AABAE0DA86BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" r:id="rId1"/>
+    <sheet name="Deployments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Subscription</t>
   </si>
@@ -47,6 +48,9 @@
     <t>Azure subscription 1</t>
   </si>
   <si>
+    <t>Subscription slug</t>
+  </si>
+  <si>
     <t>rg-pulumi-nvtst</t>
   </si>
   <si>
@@ -54,6 +58,33 @@
   </si>
   <si>
     <t>stpuluminvtst</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Resource Group</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>Defines</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>rg-nvdev-uks</t>
+  </si>
+  <si>
+    <t>nv1</t>
   </si>
 </sst>
 </file>
@@ -405,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B5BE03-3E04-4B25-A092-09DC9FC1B466}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,18 +458,76 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D64D179-1202-49C2-AB69-A35012CE5234}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>